<commit_message>
Add the link to new documentation
</commit_message>
<xml_diff>
--- a/src/_static/xlsx/tab_Cessazione_unione_civile___convivenze.xlsx
+++ b/src/_static/xlsx/tab_Cessazione_unione_civile___convivenze.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="0" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="510" windowWidth="20700" windowHeight="10935"/>
+    <workbookView xWindow="630" yWindow="510" windowWidth="19440" windowHeight="10935"/>
   </bookViews>
   <sheets>
     <sheet name="Tabella 31" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Sentenza</t>
-  </si>
-  <si>
-    <t>Matrimonio</t>
   </si>
   <si>
     <t>Accordo tra le parti</t>
@@ -400,11 +397,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -459,7 +456,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -467,7 +464,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -475,7 +472,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -483,18 +480,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>98</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -504,9 +493,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -624,25 +616,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3958BE9-611C-4D19-857D-1F92BB9E65A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64B5B95B-2806-47FC-8913-0A0107E842D6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -664,9 +646,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64B5B95B-2806-47FC-8913-0A0107E842D6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3958BE9-611C-4D19-857D-1F92BB9E65A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
link updated on 20190308
</commit_message>
<xml_diff>
--- a/src/_static/xlsx/tab_Cessazione_unione_civile___convivenze.xlsx
+++ b/src/_static/xlsx/tab_Cessazione_unione_civile___convivenze.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="0" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="510" windowWidth="19440" windowHeight="10935"/>
+    <workbookView xWindow="630" yWindow="570" windowWidth="19440" windowHeight="10875"/>
   </bookViews>
   <sheets>
     <sheet name="Tabella 31" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>Decesso del convivente/unito civilmente</t>
+  </si>
+  <si>
+    <t>31,32,34 utilizzati per convivenze di fatto</t>
+  </si>
+  <si>
+    <t>98 utilizzato in entrambi i casi</t>
+  </si>
+  <si>
+    <t>1,2,3 utilizzati per unioni civili</t>
   </si>
 </sst>
 </file>
@@ -397,11 +406,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -484,6 +493,21 @@
       </c>
       <c r="B8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -649,13 +673,13 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3958BE9-611C-4D19-857D-1F92BB9E65A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>